<commit_message>
correcao do problema para atualizar o mapa antes de exibir.
</commit_message>
<xml_diff>
--- a/assets/planilhas/promocoes.xlsx
+++ b/assets/planilhas/promocoes.xlsx
@@ -22,12 +22,12 @@
     </font>
     <font>
       <name val="Arial"/>
-      <color rgb="FF000000"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
     </font>
     <font>
       <name val="Arial"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -50,28 +50,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -348,7 +341,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,9 +349,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="19.63" customWidth="1" style="7" min="2" max="2"/>
-    <col width="19.5" customWidth="1" style="7" min="3" max="3"/>
-    <col width="19.63" customWidth="1" style="7" min="4" max="5"/>
+    <col width="19.38" customWidth="1" style="6" min="1" max="1"/>
+    <col width="22.63" customWidth="1" style="6" min="2" max="2"/>
+    <col width="22.25" customWidth="1" style="6" min="4" max="4"/>
+    <col width="22" customWidth="1" style="6" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -404,14 +398,14 @@
           <t>20%</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>-29.699.552.440.195.800</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>-52.437.911.713.362.900</t>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>-29.6995524401958</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>-52.4379117133629</t>
         </is>
       </c>
     </row>
@@ -431,14 +425,14 @@
           <t>5%</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>-29.725.230.540.229.800</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>-52.42700418680375</t>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>-29.7252305402298</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>-52.4270041868037</t>
         </is>
       </c>
     </row>
@@ -458,14 +452,14 @@
           <t>8%</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>-29.718.477.199.300.200</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>-52.429.675.627.956.900</t>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>-29.7184771993002</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>-52.4296756279569</t>
         </is>
       </c>
     </row>
@@ -485,347 +479,411 @@
           <t>10%</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>-29.714727978452064</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>-52.42951154653881</t>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>-29.7147279784521</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>-52.4295115465388</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Convés</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Hambúrgueres</t>
+          <t>Mundo Animal</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Torres de batata</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>15%</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>-29.711213851183132</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>-52.42971265463833</t>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>-29.709187307988</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>-52.4262553351454</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>FNP</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>Potchês</t>
+          <t>Convés</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Hambúrgueres</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>25%</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>-29.718594009988493</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>-52.42456347461825</t>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>-29.7112138511831</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>-52.4297126546383</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Brolese</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Rodízio</t>
+          <t>FNP</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Potchês</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>40%</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>-29.702953088222753</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>-52.43039916503408</t>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>-29.7185940099885</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>-52.4245634746182</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Dog Center</t>
+          <t>Brolese</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>Dog's</t>
+          <t>Rodízio</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>-29.71856970395839</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>-52.42740497407137</t>
+          <t>40%</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>-29.7029530882228</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr">
+        <is>
+          <t>-52.4303991650340</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Subway</t>
+          <t>Dog Center</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>Sub Big Boss</t>
+          <t>Dog's</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>-29.714558186330635</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>-52.42745370475684</t>
+          <t>10%</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>-29.7185697039584</t>
+        </is>
+      </c>
+      <c r="E10" s="5" t="inlineStr">
+        <is>
+          <t>-52.4274049740713</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Mc Donald's</t>
-        </is>
-      </c>
-      <c r="B11" s="6" t="inlineStr">
-        <is>
-          <t>Quarterão com Queijo</t>
+          <t>Subway</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Sub Big Boss</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>40%</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>-29.716402599735016</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>-52.42564265263388</t>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>-29.7145581863306</t>
+        </is>
+      </c>
+      <c r="E11" s="5" t="inlineStr">
+        <is>
+          <t>-52.4274537047568</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Giraffas</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>Girabox</t>
+          <t>Mc Donald's</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>Quarterão com Queijo</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>20%</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>-29.715801870252886</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>-52.424925020099266</t>
+          <t>40%</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>-29.7164025997350</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t>-52.4256426526338</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Quiero Café</t>
+          <t>Giraffas</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>Massas</t>
+          <t>Girabox</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>12%</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>-29.715.801.870.252.800</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>-52.424.925.020.099.200</t>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>-29.7158018702529</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t>-52.4249250200992</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Sorella</t>
+          <t>Quiero Café</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>Waffles</t>
+          <t>Massas</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>-29.704138906633556</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>-52.428638111946384</t>
+          <t>12%</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>-29.7158018702528</t>
+        </is>
+      </c>
+      <c r="E14" s="5" t="inlineStr">
+        <is>
+          <t>-52.4249250200992</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
+          <t>Sorella</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Waffles</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>-29.7041389066336</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr">
+        <is>
+          <t>-52.4286381119463</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
           <t>Jamaica</t>
         </is>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>Sonho</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>10%</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>-29.716.811.053.269.000</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="inlineStr">
-        <is>
-          <t>-52.429.490.511.974.100</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="inlineStr">
-        <is>
-          <t>Mundo Animal</t>
-        </is>
-      </c>
-      <c r="B16" s="0" t="inlineStr">
-        <is>
-          <t>Torres de batata</t>
-        </is>
-      </c>
-      <c r="C16" s="0" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="D16" s="0" t="inlineStr">
-        <is>
-          <t>-29.709187307987996</t>
-        </is>
-      </c>
-      <c r="E16" s="0" t="inlineStr">
-        <is>
-          <t>-52.42625533514549</t>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t>-29.7168110532690</t>
+        </is>
+      </c>
+      <c r="E16" s="5" t="inlineStr">
+        <is>
+          <t>-52.4294905119741</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-      <c r="B17" s="0" t="inlineStr">
-        <is>
-          <t>testes</t>
-        </is>
-      </c>
-      <c r="C17" s="0" t="inlineStr">
+      <c r="D17" s="5" t="n"/>
+      <c r="E17" s="5" t="n"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="5" t="n"/>
+      <c r="E18" s="5" t="n"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="5" t="n"/>
+      <c r="E19" s="5" t="n"/>
+    </row>
+    <row r="20">
+      <c r="D20" s="5" t="n"/>
+      <c r="E20" s="5" t="n"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="5" t="n"/>
+      <c r="E21" s="5" t="n"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="5" t="n"/>
+      <c r="E22" s="5" t="n"/>
+    </row>
+    <row r="23">
+      <c r="D23" s="5" t="n"/>
+      <c r="E23" s="5" t="n"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="5" t="n"/>
+      <c r="E24" s="5" t="n"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="5" t="n"/>
+      <c r="E25" s="5" t="n"/>
+    </row>
+    <row r="26">
+      <c r="D26" s="5" t="n"/>
+      <c r="E26" s="5" t="n"/>
+    </row>
+    <row r="27">
+      <c r="D27" s="5" t="n"/>
+      <c r="E27" s="5" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>DFSUL fiat</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>Carro</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>-29.70242815091569</t>
+        </is>
+      </c>
+      <c r="E28" s="0" t="inlineStr">
+        <is>
+          <t>-52.44654570731936</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Lojas Renner</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Camisetas</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="D17" s="0" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="E17" s="0" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>-29.715169145860852</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-52.42794732804669</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>